<commit_message>
Created working XML file using vignette and EDIutil functions still needs more organization and text fixes
</commit_message>
<xml_diff>
--- a/data-raw/Hannon-Example/example-metadata.xlsx
+++ b/data-raw/Hannon-Example/example-metadata.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\EDIutils\data-raw\Hannon-Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2465E27D-E71C-42DF-9428-CB78601F263F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3255A3D7-7499-4341-AA97-AD4EB1FC4156}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-12615" windowWidth="29040" windowHeight="15840" tabRatio="834" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15570" yWindow="-13905" windowWidth="26160" windowHeight="10710" tabRatio="834" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="personnel" sheetId="1" r:id="rId1"/>
     <sheet name="title" sheetId="2" r:id="rId2"/>
     <sheet name="keyword_set" sheetId="3" r:id="rId3"/>
     <sheet name="license" sheetId="4" r:id="rId4"/>
-    <sheet name="funding" sheetId="5" r:id="rId5"/>
-    <sheet name="project_title" sheetId="11" r:id="rId6"/>
+    <sheet name="project_title" sheetId="11" r:id="rId5"/>
+    <sheet name="funding" sheetId="5" r:id="rId6"/>
     <sheet name="project_personnel" sheetId="12" r:id="rId7"/>
     <sheet name="maintenance" sheetId="6" r:id="rId8"/>
     <sheet name="coverage" sheetId="7" r:id="rId9"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="177">
   <si>
     <t>first_name</t>
   </si>
@@ -311,9 +311,6 @@
     <t>length</t>
   </si>
   <si>
-    <t>NEED HELP HERE</t>
-  </si>
-  <si>
     <t>treatment</t>
   </si>
   <si>
@@ -359,9 +356,6 @@
     <t>real</t>
   </si>
   <si>
-    <t>visibility</t>
-  </si>
-  <si>
     <t>survey_method</t>
   </si>
   <si>
@@ -410,9 +404,6 @@
     <t>adult_predator_fish</t>
   </si>
   <si>
-    <t>count of fissh that were naturak predators</t>
-  </si>
-  <si>
     <t>other_juvenile_fish</t>
   </si>
   <si>
@@ -425,9 +416,6 @@
     <t>estimated flow in cubic feet per second</t>
   </si>
   <si>
-    <t>interger</t>
-  </si>
-  <si>
     <t>code</t>
   </si>
   <si>
@@ -503,31 +491,82 @@
     <t>observer counted</t>
   </si>
   <si>
-    <t>CVPIA</t>
-  </si>
-  <si>
     <t>CCO</t>
   </si>
   <si>
     <t>project_title</t>
   </si>
   <si>
-    <t xml:space="preserve">Hannon Project </t>
-  </si>
-  <si>
     <t xml:space="preserve">Any additional comments describing the data collected </t>
   </si>
   <si>
     <t>storage_type</t>
   </si>
   <si>
-    <t xml:space="preserve">taken in feet using a secchi disk </t>
-  </si>
-  <si>
     <t>dbl</t>
   </si>
   <si>
     <t>string</t>
+  </si>
+  <si>
+    <t>BCWC</t>
+  </si>
+  <si>
+    <t>program founder</t>
+  </si>
+  <si>
+    <t>CVPIA_common_species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nominal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ratio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">numeric </t>
+  </si>
+  <si>
+    <t>meter</t>
+  </si>
+  <si>
+    <t>cubicFeetPerSecond</t>
+  </si>
+  <si>
+    <t>natural</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The water level on the day the data was collected </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The length of the site sampled </t>
+  </si>
+  <si>
+    <t>count of fish that were natural predators</t>
+  </si>
+  <si>
+    <t>other fish counted</t>
+  </si>
+  <si>
+    <t>visibility_feet</t>
+  </si>
+  <si>
+    <t>visibility_meters</t>
+  </si>
+  <si>
+    <t>The visability converted to meters</t>
+  </si>
+  <si>
+    <t>CVPIA Salmonid Habitat Monitoring Project</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The visability in feet measeured using a secchi disk </t>
+  </si>
+  <si>
+    <t>foot</t>
   </si>
 </sst>
 </file>
@@ -572,12 +611,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -593,10 +638,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -609,6 +653,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -995,14 +1046,15 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18.875" customWidth="1"/>
-    <col min="5" max="5" width="27.375" customWidth="1"/>
-    <col min="6" max="6" width="27" customWidth="1"/>
+    <col min="5" max="5" width="27" customWidth="1"/>
+    <col min="6" max="6" width="27.375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1019,10 +1071,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1038,11 +1090,11 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1056,10 +1108,10 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" t="s">
+      <c r="E3" t="s">
         <v>15</v>
       </c>
+      <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1071,6 +1123,9 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
+      <c r="E4" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1082,7 +1137,7 @@
       <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1103,60 +1158,69 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.375" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="8" max="8" width="10.375" customWidth="1"/>
-    <col min="9" max="9" width="32.625" customWidth="1"/>
+    <col min="1" max="1" width="21.25" customWidth="1"/>
+    <col min="2" max="2" width="13.375" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="9" max="9" width="10.375" customWidth="1"/>
+    <col min="10" max="10" width="32.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" t="s">
         <v>56</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>58</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>59</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>60</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>61</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>62</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>63</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A8" xr:uid="{E84463C8-B007-49D1-B1DB-07F049FCEC34}">
+      <formula1>"chinook, delta_smelt, steelhead, white_sturgeon, green_sturgeon"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -1164,516 +1228,646 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AMH21"/>
+  <dimension ref="A1:AMH22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="19.75" style="3"/>
-    <col min="3" max="3" width="13.125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="17.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="13.25" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="5.375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="5.625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.25" style="3" customWidth="1"/>
-    <col min="10" max="10" width="11.75" style="3" customWidth="1"/>
-    <col min="11" max="11" width="16" style="3" customWidth="1"/>
-    <col min="12" max="12" width="17.625" style="3" customWidth="1"/>
-    <col min="13" max="14" width="9.25" style="3" customWidth="1"/>
-    <col min="15" max="1022" width="19.75" style="3"/>
+    <col min="1" max="2" width="19.75" style="2"/>
+    <col min="3" max="3" width="13.125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="17.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.25" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.25" style="2" customWidth="1"/>
+    <col min="8" max="8" width="20.75" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.25" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.875" style="12" customWidth="1"/>
+    <col min="11" max="11" width="16" style="2" customWidth="1"/>
+    <col min="12" max="12" width="17.625" style="2" customWidth="1"/>
+    <col min="13" max="14" width="9.25" style="2" customWidth="1"/>
+    <col min="15" max="1022" width="19.75" style="2"/>
     <col min="1023" max="1025" width="8.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M2" s="6">
+        <v>42019</v>
+      </c>
+      <c r="N2" s="6">
+        <v>43496</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="63" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="63" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="M5" s="2">
+        <v>88</v>
+      </c>
+      <c r="N5" s="2">
+        <v>3526</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="N8" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M10" s="2">
+        <v>44</v>
+      </c>
+      <c r="N10" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+      <c r="N11" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="N12" s="2">
+        <v>3.66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2">
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0</v>
+      </c>
+      <c r="N16" s="2">
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0</v>
+      </c>
+      <c r="N17" s="2">
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+      <c r="N18" s="2">
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="M19" s="2">
+        <v>0</v>
+      </c>
+      <c r="N19" s="2">
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="M20" s="2">
+        <v>0</v>
+      </c>
+      <c r="N20" s="2">
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="M2" s="7">
-        <v>42346</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="63" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="63" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D10" s="3" t="s">
+    <row r="22" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="H10" s="8" t="s">
+      <c r="G22" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="I10" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="M10" s="3">
-        <v>-100</v>
-      </c>
-      <c r="N10" s="3">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="N11" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="M14" s="3">
+      <c r="M22" s="2">
         <v>0</v>
       </c>
-      <c r="N14" s="3">
-        <v>100000000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="M15" s="3">
-        <v>0</v>
-      </c>
-      <c r="N15" s="3">
-        <v>100000000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="M16" s="3">
-        <v>0</v>
-      </c>
-      <c r="N16" s="3">
-        <v>100000000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="M17" s="3">
-        <v>0</v>
-      </c>
-      <c r="N17" s="3">
-        <v>100000000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="M21" s="3">
-        <v>0</v>
-      </c>
-      <c r="N21" s="3">
+      <c r="N22" s="2">
         <v>10000000</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1021" xr:uid="{00000000-0002-0000-0800-000000000000}">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1022" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1021" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2" xr:uid="{4F62B5AD-D3AC-4B0B-B0D2-B82A9D8B2D70}">
+      <formula1>M2</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576" xr:uid="{2CE87812-AA0D-45D0-B03C-D32D988BF082}">
+      <formula1>"whole, real, integer, natural"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F10 F12:F1022" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1021" xr:uid="{00000000-0002-0000-0800-000002000000}">
-      <formula1>"natural,whole,interger,real"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1021" xr:uid="{00000000-0002-0000-0800-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G10 G12:G1022" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>"ratio,interval"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1688,7 +1882,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1700,13 +1894,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1714,10 +1908,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1725,10 +1919,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1736,10 +1930,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1747,10 +1941,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1758,10 +1952,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1769,120 +1963,120 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B8" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B9" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B10" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B11" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B12" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B13" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B14" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B15" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C16" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B17" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C17" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1896,7 +2090,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1914,7 +2108,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B2" t="s">
@@ -1932,20 +2126,20 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46.625" customWidth="1"/>
-    <col min="2" max="2" width="22.375" customWidth="1"/>
+    <col min="2" max="2" width="22.375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1953,24 +2147,15 @@
       <c r="A2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s">
-        <v>155</v>
-      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="B3" t="s">
-        <v>155</v>
-      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
-      </c>
-      <c r="B4" t="s">
-        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1984,7 +2169,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2014,7 +2199,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2024,57 +2209,83 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CC0791-3488-4AA1-946D-D16C61358F1D}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="15.625" customWidth="1"/>
-    <col min="3" max="3" width="13.625" customWidth="1"/>
+    <col min="2" max="2" width="15.625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="13.625" style="8" customWidth="1"/>
     <col min="4" max="4" width="21.625" customWidth="1"/>
-    <col min="6" max="6" width="17.375" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="8"/>
+    <col min="6" max="6" width="17.375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="11" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="63" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="12">
         <v>12345</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -2088,40 +2299,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CC0791-3488-4AA1-946D-D16C61358F1D}">
-  <dimension ref="A1:A2"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B393E3-5912-4740-8F4D-04368D7963D5}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B393E3-5912-4740-8F4D-04368D7963D5}">
-  <dimension ref="A1:F5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.875" customWidth="1"/>
+    <col min="2" max="2" width="12.875" customWidth="1"/>
+    <col min="3" max="3" width="16.625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="16.125" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="21.375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="21.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2130,17 +2325,17 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2150,59 +2345,22 @@
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
+      <c r="C3" s="10"/>
+      <c r="F3" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -2220,10 +2378,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2231,15 +2389,18 @@
     <col min="2" max="2" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>44</v>
       </c>
       <c r="B1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -2264,7 +2425,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2300,33 +2461,38 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>-122.448217</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>-121.48444600000001</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>40.612354000000003</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>38.509402000000001</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <v>42370</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>46</v>
+      <c r="G2" s="6">
+        <v>43496</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G3" s="6"/>
+      <c r="G3" s="5"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{44AF0CB8-82BE-41E6-9D41-85F632723101}">
+      <formula1>F2</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
Removed description from maintenance because status becomes the description
</commit_message>
<xml_diff>
--- a/data-raw/Hannon-Example/example-metadata.xlsx
+++ b/data-raw/Hannon-Example/example-metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\EDIutils\data-raw\Hannon-Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3255A3D7-7499-4341-AA97-AD4EB1FC4156}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0AA1FD-8B29-42A3-AC78-9260A96EAD3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15570" yWindow="-13905" windowWidth="26160" windowHeight="10710" tabRatio="834" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15570" yWindow="-13905" windowWidth="26160" windowHeight="10710" tabRatio="834" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="personnel" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="176">
   <si>
     <t>first_name</t>
   </si>
@@ -558,9 +558,6 @@
   </si>
   <si>
     <t>CVPIA Salmonid Habitat Monitoring Project</t>
-  </si>
-  <si>
-    <t>description</t>
   </si>
   <si>
     <t xml:space="preserve">The visability in feet measeured using a secchi disk </t>
@@ -1230,7 +1227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMH22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -1517,7 +1514,7 @@
         <v>170</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>155</v>
@@ -1532,7 +1529,7 @@
         <v>102</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>105</v>
@@ -2378,10 +2375,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2389,18 +2386,15 @@
     <col min="2" max="2" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>44</v>
       </c>
       <c r="B1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
Fix metadata excel and csv so that it passes all EDI tests
</commit_message>
<xml_diff>
--- a/data-raw/Hannon-Example/example-metadata.xlsx
+++ b/data-raw/Hannon-Example/example-metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\EDIutils\data-raw\Hannon-Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0AA1FD-8B29-42A3-AC78-9260A96EAD3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED50C06-3E65-4304-A9E8-7F1384352B8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15570" yWindow="-13905" windowWidth="26160" windowHeight="10710" tabRatio="834" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12510" yWindow="-12135" windowWidth="21600" windowHeight="11385" tabRatio="834" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="personnel" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="attribute" sheetId="9" r:id="rId11"/>
     <sheet name="code_definitions" sheetId="10" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="182">
   <si>
     <t>first_name</t>
   </si>
@@ -564,6 +564,24 @@
   </si>
   <si>
     <t>foot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">month </t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>Month in which data was collected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year in which data was collected </t>
+  </si>
+  <si>
+    <t>wr_count</t>
+  </si>
+  <si>
+    <t>winter run counted</t>
   </si>
 </sst>
 </file>
@@ -1225,11 +1243,9 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AMH22"/>
+  <dimension ref="A1:AMH25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1322,78 +1338,65 @@
         <v>43496</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>84</v>
+        <v>176</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>86</v>
+        <v>160</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="63" x14ac:dyDescent="0.25">
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+    </row>
+    <row r="4" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>88</v>
+        <v>177</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>86</v>
+        <v>160</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+    </row>
+    <row r="5" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>167</v>
+        <v>85</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>155</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>161</v>
+        <v>86</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="M5" s="2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="63" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="N5" s="2">
-        <v>3526</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="B6" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>156</v>
@@ -1402,281 +1405,266 @@
         <v>86</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>95</v>
+        <v>167</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>94</v>
+        <v>155</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>82</v>
+        <v>161</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>96</v>
+        <v>162</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="M7" s="2">
+        <v>88</v>
+      </c>
+      <c r="N7" s="2">
+        <v>3526</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M8" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="N8" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>155</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>103</v>
+        <v>162</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>104</v>
+        <v>112</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>105</v>
       </c>
       <c r="M10" s="2">
-        <v>44</v>
+        <v>0.4</v>
       </c>
       <c r="N10" s="2">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>170</v>
+        <v>98</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>174</v>
+        <v>99</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>155</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M11" s="2">
-        <v>0</v>
-      </c>
-      <c r="N11" s="2">
-        <v>12</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>171</v>
+        <v>100</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>172</v>
+        <v>101</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>155</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>162</v>
+        <v>103</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>163</v>
+        <v>102</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>104</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>105</v>
       </c>
       <c r="M12" s="2">
+        <v>44</v>
+      </c>
+      <c r="N12" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M14" s="2">
         <v>0.45</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N14" s="2">
         <v>3.66</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="15" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C15" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="M15" s="2">
-        <v>0</v>
-      </c>
-      <c r="N15" s="2">
-        <v>100000000</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="M16" s="2">
-        <v>0</v>
-      </c>
-      <c r="N16" s="2">
-        <v>100000000</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>155</v>
@@ -1705,10 +1693,10 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>119</v>
+        <v>180</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>120</v>
+        <v>181</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>155</v>
@@ -1735,12 +1723,12 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>168</v>
+        <v>116</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>155</v>
@@ -1769,10 +1757,10 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>169</v>
+        <v>118</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>155</v>
@@ -1799,29 +1787,44 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>153</v>
+        <v>120</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>160</v>
+        <v>112</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>87</v>
+        <v>103</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="M21" s="2">
+        <v>0</v>
+      </c>
+      <c r="N21" s="2">
+        <v>100000000</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>125</v>
+        <v>168</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>155</v>
@@ -1836,35 +1839,116 @@
         <v>112</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>164</v>
+        <v>113</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="M22" s="2">
         <v>0</v>
       </c>
       <c r="N22" s="2">
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+      <c r="N23" s="2">
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M25" s="2">
+        <v>0</v>
+      </c>
+      <c r="N25" s="2">
         <v>10000000</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1022" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1025" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2" xr:uid="{4F62B5AD-D3AC-4B0B-B0D2-B82A9D8B2D70}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N4" xr:uid="{4F62B5AD-D3AC-4B0B-B0D2-B82A9D8B2D70}">
       <formula1>M2</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576" xr:uid="{2CE87812-AA0D-45D0-B03C-D32D988BF082}">
       <formula1>"whole, real, integer, natural"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F10 F12:F1022" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F12 F14:F1025" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G10 G12:G1022" xr:uid="{00000000-0002-0000-0800-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G12 G14:G1025" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>"ratio,interval"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2377,7 +2461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Improved code for taxonomic classifcation and added access
</commit_message>
<xml_diff>
--- a/data-raw/Hannon-Example/example-metadata.xlsx
+++ b/data-raw/Hannon-Example/example-metadata.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\EDIutils\data-raw\Hannon-Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED50C06-3E65-4304-A9E8-7F1384352B8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B51AF5C-6DAC-4C71-ADBB-7BEFD4233B4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12510" yWindow="-12135" windowWidth="21600" windowHeight="11385" tabRatio="834" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11670" yWindow="-14985" windowWidth="25230" windowHeight="13560" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="personnel" sheetId="1" r:id="rId1"/>
-    <sheet name="title" sheetId="2" r:id="rId2"/>
-    <sheet name="keyword_set" sheetId="3" r:id="rId3"/>
-    <sheet name="license" sheetId="4" r:id="rId4"/>
-    <sheet name="project_title" sheetId="11" r:id="rId5"/>
-    <sheet name="funding" sheetId="5" r:id="rId6"/>
-    <sheet name="project_personnel" sheetId="12" r:id="rId7"/>
-    <sheet name="maintenance" sheetId="6" r:id="rId8"/>
-    <sheet name="coverage" sheetId="7" r:id="rId9"/>
-    <sheet name="taxonomic_coverage" sheetId="8" r:id="rId10"/>
-    <sheet name="attribute" sheetId="9" r:id="rId11"/>
-    <sheet name="code_definitions" sheetId="10" r:id="rId12"/>
+    <sheet name="dataset" sheetId="13" r:id="rId1"/>
+    <sheet name="personnel" sheetId="1" r:id="rId2"/>
+    <sheet name="title" sheetId="2" r:id="rId3"/>
+    <sheet name="keyword_set" sheetId="3" r:id="rId4"/>
+    <sheet name="license" sheetId="4" r:id="rId5"/>
+    <sheet name="project_title" sheetId="11" r:id="rId6"/>
+    <sheet name="funding" sheetId="5" r:id="rId7"/>
+    <sheet name="project_personnel" sheetId="12" r:id="rId8"/>
+    <sheet name="maintenance" sheetId="6" r:id="rId9"/>
+    <sheet name="coverage" sheetId="7" r:id="rId10"/>
+    <sheet name="taxonomic_coverage" sheetId="8" r:id="rId11"/>
+    <sheet name="attribute" sheetId="9" r:id="rId12"/>
+    <sheet name="code_definitions" sheetId="10" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="186">
   <si>
     <t>first_name</t>
   </si>
@@ -582,6 +583,18 @@
   </si>
   <si>
     <t>winter run counted</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geometry </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hannon Salmonid Survey Data </t>
+  </si>
+  <si>
+    <t>tabular</t>
   </si>
 </sst>
 </file>
@@ -1057,121 +1070,118 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2431AD77-9C3B-495F-B247-9D17815BE20F}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.875" customWidth="1"/>
-    <col min="5" max="5" width="27" customWidth="1"/>
-    <col min="6" max="6" width="27.375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="27" customWidth="1"/>
+    <col min="1" max="1" width="26.125" customWidth="1"/>
+    <col min="2" max="2" width="23.875" customWidth="1"/>
+    <col min="3" max="3" width="22.625" customWidth="1"/>
+    <col min="4" max="4" width="24.125" customWidth="1"/>
+    <col min="5" max="5" width="23.875" customWidth="1"/>
+    <col min="8" max="8" width="53.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="10"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="2">
+        <v>-122.448217</v>
+      </c>
+      <c r="C2" s="2">
+        <v>-121.48444600000001</v>
+      </c>
+      <c r="D2" s="2">
+        <v>40.612354000000003</v>
+      </c>
+      <c r="E2" s="2">
+        <v>38.509402000000001</v>
+      </c>
+      <c r="F2" s="5">
+        <v>42370</v>
+      </c>
+      <c r="G2" s="6">
+        <v>43496</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1005" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>"creator,field technician,program founder,other,associate,reviewer,researcher,principal investigator,lab technician"</formula1>
-      <formula2>0</formula2>
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{44AF0CB8-82BE-41E6-9D41-85F632723101}">
+      <formula1>F2</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -1241,11 +1251,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMH25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1958,7 +1968,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -2167,6 +2177,121 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.875" customWidth="1"/>
+    <col min="5" max="5" width="27" customWidth="1"/>
+    <col min="6" max="6" width="27.375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1005" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>"creator,field technician,program founder,other,associate,reviewer,researcher,principal investigator,lab technician"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2202,7 +2327,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -2245,7 +2370,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2289,7 +2414,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CC0791-3488-4AA1-946D-D16C61358F1D}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2314,7 +2439,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -2380,7 +2505,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B393E3-5912-4740-8F4D-04368D7963D5}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2457,7 +2582,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2496,82 +2621,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.125" customWidth="1"/>
-    <col min="2" max="2" width="23.875" customWidth="1"/>
-    <col min="3" max="3" width="22.625" customWidth="1"/>
-    <col min="4" max="4" width="24.125" customWidth="1"/>
-    <col min="5" max="5" width="23.875" customWidth="1"/>
-    <col min="8" max="8" width="53.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="2">
-        <v>-122.448217</v>
-      </c>
-      <c r="C2" s="2">
-        <v>-121.48444600000001</v>
-      </c>
-      <c r="D2" s="2">
-        <v>40.612354000000003</v>
-      </c>
-      <c r="E2" s="2">
-        <v>38.509402000000001</v>
-      </c>
-      <c r="F2" s="5">
-        <v>42370</v>
-      </c>
-      <c r="G2" s="6">
-        <v>43496</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G3" s="5"/>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{44AF0CB8-82BE-41E6-9D41-85F632723101}">
-      <formula1>F2</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
reformated creating-EML to make working XML with EDI number
</commit_message>
<xml_diff>
--- a/data-raw/Hannon-Example/example-metadata.xlsx
+++ b/data-raw/Hannon-Example/example-metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\EDIutils\data-raw\Hannon-Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B51AF5C-6DAC-4C71-ADBB-7BEFD4233B4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600932CA-8A7D-4C45-A3BA-2A8CC1F862F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11670" yWindow="-14985" windowWidth="25230" windowHeight="13560" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" tabRatio="834" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -18,14 +18,13 @@
     <sheet name="title" sheetId="2" r:id="rId3"/>
     <sheet name="keyword_set" sheetId="3" r:id="rId4"/>
     <sheet name="license" sheetId="4" r:id="rId5"/>
-    <sheet name="project_title" sheetId="11" r:id="rId6"/>
+    <sheet name="project" sheetId="11" r:id="rId6"/>
     <sheet name="funding" sheetId="5" r:id="rId7"/>
-    <sheet name="project_personnel" sheetId="12" r:id="rId8"/>
-    <sheet name="maintenance" sheetId="6" r:id="rId9"/>
-    <sheet name="coverage" sheetId="7" r:id="rId10"/>
-    <sheet name="taxonomic_coverage" sheetId="8" r:id="rId11"/>
-    <sheet name="attribute" sheetId="9" r:id="rId12"/>
-    <sheet name="code_definitions" sheetId="10" r:id="rId13"/>
+    <sheet name="maintenance" sheetId="6" r:id="rId8"/>
+    <sheet name="coverage" sheetId="7" r:id="rId9"/>
+    <sheet name="taxonomic_coverage" sheetId="8" r:id="rId10"/>
+    <sheet name="attribute" sheetId="9" r:id="rId11"/>
+    <sheet name="code_definitions" sheetId="10" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1073,7 +1072,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2431AD77-9C3B-495F-B247-9D17815BE20F}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -1104,84 +1103,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.125" customWidth="1"/>
-    <col min="2" max="2" width="23.875" customWidth="1"/>
-    <col min="3" max="3" width="22.625" customWidth="1"/>
-    <col min="4" max="4" width="24.125" customWidth="1"/>
-    <col min="5" max="5" width="23.875" customWidth="1"/>
-    <col min="8" max="8" width="53.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="2">
-        <v>-122.448217</v>
-      </c>
-      <c r="C2" s="2">
-        <v>-121.48444600000001</v>
-      </c>
-      <c r="D2" s="2">
-        <v>40.612354000000003</v>
-      </c>
-      <c r="E2" s="2">
-        <v>38.509402000000001</v>
-      </c>
-      <c r="F2" s="5">
-        <v>42370</v>
-      </c>
-      <c r="G2" s="6">
-        <v>43496</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G3" s="5"/>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{44AF0CB8-82BE-41E6-9D41-85F632723101}">
-      <formula1>F2</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -1251,7 +1172,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMH25"/>
   <sheetViews>
@@ -1968,7 +1889,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -2416,25 +2337,82 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CC0791-3488-4AA1-946D-D16C61358F1D}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="12.875" customWidth="1"/>
+    <col min="4" max="4" width="16.625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="16.125" customWidth="1"/>
+    <col min="6" max="6" width="21.5" customWidth="1"/>
+    <col min="7" max="7" width="21.375" style="8" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>173</v>
       </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D3" s="10"/>
+      <c r="G3" s="10"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E5" xr:uid="{87D8C41F-E5D3-4B3A-821F-C374ECE1C22E}">
+      <formula1>"creator,field technician,program founder,other,associate,reviewer,researcher,principal investigator,lab technician"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{7EED9AF2-05B0-4782-BF99-E71B1E85279C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2506,88 +2484,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B393E3-5912-4740-8F4D-04368D7963D5}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.875" customWidth="1"/>
-    <col min="2" max="2" width="12.875" customWidth="1"/>
-    <col min="3" max="3" width="16.625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="16.125" customWidth="1"/>
-    <col min="5" max="5" width="21.5" customWidth="1"/>
-    <col min="6" max="6" width="21.375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="21.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="10"/>
-      <c r="F3" s="10"/>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D5" xr:uid="{495ACF41-C572-43B5-B373-8A75A2744707}">
-      <formula1>"creator,field technician,program founder,other,associate,reviewer,researcher,principal investigator,lab technician"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{515BD050-7D95-47EE-96DB-B50D1B9E685C}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2621,4 +2522,82 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.125" customWidth="1"/>
+    <col min="2" max="2" width="23.875" customWidth="1"/>
+    <col min="3" max="3" width="22.625" customWidth="1"/>
+    <col min="4" max="4" width="24.125" customWidth="1"/>
+    <col min="5" max="5" width="23.875" customWidth="1"/>
+    <col min="8" max="8" width="53.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="2">
+        <v>-122.448217</v>
+      </c>
+      <c r="C2" s="2">
+        <v>-121.48444600000001</v>
+      </c>
+      <c r="D2" s="2">
+        <v>40.612354000000003</v>
+      </c>
+      <c r="E2" s="2">
+        <v>38.509402000000001</v>
+      </c>
+      <c r="F2" s="5">
+        <v>42370</v>
+      </c>
+      <c r="G2" s="6">
+        <v>43496</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="5"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{44AF0CB8-82BE-41E6-9D41-85F632723101}">
+      <formula1>F2</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added tests for default funding options
</commit_message>
<xml_diff>
--- a/data-raw/Hannon-Example/example-metadata.xlsx
+++ b/data-raw/Hannon-Example/example-metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\EDIutils\data-raw\Hannon-Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600932CA-8A7D-4C45-A3BA-2A8CC1F862F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BF0F7E-DB3A-4472-8ED0-CC2BBF42121C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" tabRatio="834" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2145" yWindow="975" windowWidth="15375" windowHeight="7875" tabRatio="834" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="187">
   <si>
     <t>first_name</t>
   </si>
@@ -594,6 +594,9 @@
   </si>
   <si>
     <t>tabular</t>
+  </si>
+  <si>
+    <t>CVPIA_default_funder</t>
   </si>
 </sst>
 </file>
@@ -2339,7 +2342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CC0791-3488-4AA1-946D-D16C61358F1D}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -2419,63 +2422,70 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="15.625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="13.625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="21.625" customWidth="1"/>
-    <col min="5" max="5" width="10.5" style="8"/>
-    <col min="6" max="6" width="17.375" style="8" customWidth="1"/>
+    <col min="1" max="1" width="21.125" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="15.625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="13.625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="21.625" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="8"/>
+    <col min="7" max="7" width="17.375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="63" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="12">
+      <c r="D2" s="12">
         <v>12345</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="12"/>
       <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1002" xr:uid="{00000000-0002-0000-0400-000000000000}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1002" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>"TBD"</formula1>
       <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{24264C25-9192-493A-B2AA-4568F5CEA44F}">
+      <formula1>"USBR, CDWR, CDFW"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Reformated add_funding defaults and tests
</commit_message>
<xml_diff>
--- a/data-raw/Hannon-Example/example-metadata.xlsx
+++ b/data-raw/Hannon-Example/example-metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\EDIutils\data-raw\Hannon-Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BF0F7E-DB3A-4472-8ED0-CC2BBF42121C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488ABB2C-E0B9-412D-905B-04F7CE7DE371}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2145" yWindow="975" windowWidth="15375" windowHeight="7875" tabRatio="834" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="186">
   <si>
     <t>first_name</t>
   </si>
@@ -594,9 +594,6 @@
   </si>
   <si>
     <t>tabular</t>
-  </si>
-  <si>
-    <t>CVPIA_default_funder</t>
   </si>
 </sst>
 </file>
@@ -2422,70 +2419,63 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.125" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="15.625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="13.625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="21.625" customWidth="1"/>
-    <col min="6" max="6" width="10.5" style="8"/>
-    <col min="7" max="7" width="17.375" style="8" customWidth="1"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="15.625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="13.625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="21.625" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="8"/>
+    <col min="6" max="6" width="17.375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="B1" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="B1" s="11" t="s">
+        <v>36</v>
+      </c>
       <c r="C1" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="E1" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="F1" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="63" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="B2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="12">
+      <c r="C2" s="12">
         <v>12345</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="E2" s="12"/>
       <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1002" xr:uid="{00000000-0002-0000-0400-000000000000}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1002" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>"TBD"</formula1>
       <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{24264C25-9192-493A-B2AA-4568F5CEA44F}">
-      <formula1>"USBR, CDWR, CDFW"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Begins edits to vignettes based on feedback from Sadie.
</commit_message>
<xml_diff>
--- a/data-raw/Hannon-Example/example-metadata.xlsx
+++ b/data-raw/Hannon-Example/example-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\EDIutils\data-raw\Hannon-Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488ABB2C-E0B9-412D-905B-04F7CE7DE371}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C8CAE4-9306-4393-913F-14656C4A6B49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="975" windowWidth="15375" windowHeight="7875" tabRatio="834" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18720" yWindow="-16410" windowWidth="29040" windowHeight="15840" tabRatio="834" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="184">
   <si>
     <t>first_name</t>
   </si>
@@ -494,9 +494,6 @@
     <t>CCO</t>
   </si>
   <si>
-    <t>project_title</t>
-  </si>
-  <si>
     <t xml:space="preserve">Any additional comments describing the data collected </t>
   </si>
   <si>
@@ -555,9 +552,6 @@
   </si>
   <si>
     <t>The visability converted to meters</t>
-  </si>
-  <si>
-    <t>CVPIA Salmonid Habitat Monitoring Project</t>
   </si>
   <si>
     <t xml:space="preserve">The visability in feet measeured using a secchi disk </t>
@@ -1080,21 +1074,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B1" t="s">
         <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -1121,7 +1115,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B1" t="s">
         <v>56</v>
@@ -1204,7 +1198,7 @@
         <v>68</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>69</v>
@@ -1248,7 +1242,7 @@
         <v>81</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>82</v>
@@ -1271,13 +1265,13 @@
     </row>
     <row r="3" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>178</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>87</v>
@@ -1289,13 +1283,13 @@
     </row>
     <row r="4" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>179</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>87</v>
@@ -1313,7 +1307,7 @@
         <v>85</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>86</v>
@@ -1330,7 +1324,7 @@
         <v>89</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>86</v>
@@ -1344,25 +1338,25 @@
         <v>90</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>112</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M7" s="2">
         <v>88</v>
@@ -1379,7 +1373,7 @@
         <v>92</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>86</v>
@@ -1416,22 +1410,22 @@
         <v>97</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>112</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>112</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>105</v>
@@ -1451,7 +1445,7 @@
         <v>99</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>86</v>
@@ -1468,7 +1462,7 @@
         <v>101</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>102</v>
@@ -1494,13 +1488,13 @@
     </row>
     <row r="13" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>112</v>
@@ -1512,7 +1506,7 @@
         <v>102</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>105</v>
@@ -1526,25 +1520,25 @@
     </row>
     <row r="14" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="C14" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>112</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>112</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>105</v>
@@ -1564,7 +1558,7 @@
         <v>107</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>86</v>
@@ -1581,7 +1575,7 @@
         <v>109</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>86</v>
@@ -1598,7 +1592,7 @@
         <v>111</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>112</v>
@@ -1624,13 +1618,13 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>112</v>
@@ -1662,7 +1656,7 @@
         <v>116</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>112</v>
@@ -1694,7 +1688,7 @@
         <v>118</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>112</v>
@@ -1726,7 +1720,7 @@
         <v>120</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>112</v>
@@ -1755,10 +1749,10 @@
         <v>121</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>112</v>
@@ -1787,10 +1781,10 @@
         <v>122</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>112</v>
@@ -1819,13 +1813,13 @@
         <v>123</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>87</v>
@@ -1839,7 +1833,7 @@
         <v>125</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>112</v>
@@ -1851,7 +1845,7 @@
         <v>112</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>105</v>
@@ -2180,7 +2174,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2337,81 +2331,75 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CC0791-3488-4AA1-946D-D16C61358F1D}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.875" customWidth="1"/>
-    <col min="3" max="3" width="12.875" customWidth="1"/>
-    <col min="4" max="4" width="16.625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="16.125" customWidth="1"/>
-    <col min="6" max="6" width="21.5" customWidth="1"/>
-    <col min="7" max="7" width="21.375" style="8" customWidth="1"/>
+    <col min="1" max="1" width="10.875" customWidth="1"/>
+    <col min="2" max="2" width="12.875" customWidth="1"/>
+    <col min="3" max="3" width="16.625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="16.125" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="21.375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>152</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
       <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>8</v>
       </c>
+      <c r="D2" t="s">
+        <v>157</v>
+      </c>
       <c r="E2" t="s">
-        <v>158</v>
-      </c>
-      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D3" s="10"/>
-      <c r="G3" s="10"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="10"/>
+      <c r="F3" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E5" xr:uid="{87D8C41F-E5D3-4B3A-821F-C374ECE1C22E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D5" xr:uid="{87D8C41F-E5D3-4B3A-821F-C374ECE1C22E}">
       <formula1>"creator,field technician,program founder,other,associate,reviewer,researcher,principal investigator,lab technician"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{7EED9AF2-05B0-4782-BF99-E71B1E85279C}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{7EED9AF2-05B0-4782-BF99-E71B1E85279C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2421,7 +2409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>